<commit_message>
table adjusted for mobile
</commit_message>
<xml_diff>
--- a/public/Documents/matches data.xlsx
+++ b/public/Documents/matches data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Srinath\Projects\IPL\IPL-master\IPL-master\public\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9050"/>
   </bookViews>
   <sheets>
     <sheet name="CSK" sheetId="3" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,16 +477,16 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -539,7 +539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -565,24 +565,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="2">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
         <v>150</v>
       </c>
       <c r="F3" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G3" s="5">
         <v>3</v>
@@ -612,12 +612,12 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>22</v>
@@ -626,7 +626,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F4" s="5">
         <v>2</v>
@@ -659,27 +659,27 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -706,7 +706,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
     </row>
   </sheetData>
@@ -722,15 +722,15 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="2"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1796875" style="2"/>
+    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -783,7 +783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -808,7 +808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="33.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="33.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>